<commit_message>
Nipah phylo analysis done
</commit_message>
<xml_diff>
--- a/Pubmed/Nipah/ReferenceSummary_Dec18.xlsx
+++ b/Pubmed/Nipah/ReferenceSummary_Dec18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/Nipah/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/Library/CloudStorage/Dropbox/Shared/___SystematicReviewsAI/Nipah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7BFBE7-A23A-7D48-B4FD-791F6D05B978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCE8BCA-4B1F-0C4E-9B21-B335E6E39487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="500" windowWidth="35220" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="37760" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1207,9 +1207,6 @@
     <t>Lung tissue samples from pigs, human samples (unspecified but likely blood)</t>
   </si>
   <si>
-    <t>Island flying foxes (Pteropus hypomelanus)</t>
-  </si>
-  <si>
     <t>1999-2000</t>
   </si>
   <si>
@@ -1528,6 +1525,9 @@
   </si>
   <si>
     <t>in GB record</t>
+  </si>
+  <si>
+    <t>Bat</t>
   </si>
 </sst>
 </file>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F75" zoomScale="91" workbookViewId="0">
-      <selection activeCell="W82" sqref="W82"/>
+    <sheetView tabSelected="1" topLeftCell="F53" zoomScale="91" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2003,7 +2003,7 @@
         <v>180</v>
       </c>
       <c r="F1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>24</v>
@@ -2012,7 +2012,7 @@
         <v>181</v>
       </c>
       <c r="I1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J1" t="s">
         <v>182</v>
@@ -2021,46 +2021,46 @@
         <v>183</v>
       </c>
       <c r="L1" t="s">
+        <v>469</v>
+      </c>
+      <c r="M1" t="s">
         <v>470</v>
       </c>
-      <c r="M1" t="s">
-        <v>471</v>
-      </c>
       <c r="N1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O1" t="s">
         <v>184</v>
       </c>
       <c r="P1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q1" t="s">
         <v>185</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -2110,7 +2110,7 @@
         <v>229</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
@@ -2185,7 +2185,7 @@
         <v>218</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>230</v>
@@ -2238,7 +2238,7 @@
         <v>204</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>197</v>
@@ -2262,7 +2262,7 @@
         <v>203</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>13</v>
@@ -2333,7 +2333,7 @@
         <v>209</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>13</v>
@@ -2407,7 +2407,7 @@
         <v>203</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>13</v>
@@ -2478,7 +2478,7 @@
         <v>203</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>13</v>
@@ -2549,7 +2549,7 @@
         <v>224</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>230</v>
@@ -2626,7 +2626,7 @@
         <v>229</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>230</v>
@@ -2703,10 +2703,10 @@
         <v>203</v>
       </c>
       <c r="P10" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>453</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>454</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>13</v>
@@ -2780,7 +2780,7 @@
         <v>241</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>230</v>
@@ -2857,7 +2857,7 @@
         <v>229</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>13</v>
@@ -2928,7 +2928,7 @@
         <v>248</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>230</v>
@@ -3005,7 +3005,7 @@
         <v>229</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>13</v>
@@ -3076,7 +3076,7 @@
         <v>229</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>13</v>
@@ -3141,7 +3141,7 @@
         <v>258</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Q16" t="s">
         <v>257</v>
@@ -3215,7 +3215,7 @@
         <v>224</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q17" s="3"/>
       <c r="R17" s="3" t="s">
@@ -3287,7 +3287,7 @@
         <v>229</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>13</v>
@@ -3358,7 +3358,7 @@
         <v>203</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>13</v>
@@ -3429,7 +3429,7 @@
         <v>203</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>13</v>
@@ -3500,7 +3500,7 @@
         <v>229</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>13</v>
@@ -3553,7 +3553,7 @@
         <v>211</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>13</v>
@@ -3603,7 +3603,7 @@
         <v>211</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>13</v>
@@ -3668,10 +3668,10 @@
         <v>229</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>13</v>
@@ -3730,10 +3730,10 @@
         <v>286</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>13</v>
@@ -3783,7 +3783,7 @@
         <v>211</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>13</v>
@@ -3854,7 +3854,7 @@
         <v>229</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>13</v>
@@ -3919,7 +3919,7 @@
         <v>203</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>13</v>
@@ -3987,7 +3987,7 @@
         <v>229</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>13</v>
@@ -4055,7 +4055,7 @@
         <v>229</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>13</v>
@@ -4123,7 +4123,7 @@
         <v>203</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>13</v>
@@ -4194,7 +4194,7 @@
         <v>303</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>230</v>
@@ -4271,7 +4271,7 @@
         <v>203</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R33" s="3" t="s">
         <v>13</v>
@@ -4342,7 +4342,7 @@
         <v>312</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>230</v>
@@ -4419,7 +4419,7 @@
         <v>203</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R35" s="3" t="s">
         <v>13</v>
@@ -4469,7 +4469,7 @@
         <v>234</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>13</v>
@@ -4540,7 +4540,7 @@
         <v>320</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R37" s="3" t="s">
         <v>13</v>
@@ -4611,7 +4611,7 @@
         <v>224</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="R38" s="3" t="s">
         <v>13</v>
@@ -4685,7 +4685,7 @@
         <v>329</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R39" s="3" t="s">
         <v>13</v>
@@ -4756,7 +4756,7 @@
         <v>224</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="R40" s="3" t="s">
         <v>13</v>
@@ -4824,7 +4824,7 @@
         <v>339</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R41" s="3" t="s">
         <v>13</v>
@@ -4898,7 +4898,7 @@
         <v>229</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R42" s="3" t="s">
         <v>13</v>
@@ -4969,7 +4969,7 @@
         <v>229</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R43" s="3" t="s">
         <v>13</v>
@@ -5019,7 +5019,7 @@
         <v>345</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="R44" s="3" t="s">
         <v>13</v>
@@ -5066,7 +5066,7 @@
         <v>346</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="R45" s="3" t="s">
         <v>13</v>
@@ -5137,7 +5137,7 @@
         <v>229</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R46" s="3" t="s">
         <v>13</v>
@@ -5184,7 +5184,7 @@
         <v>204</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="R47" s="3" t="s">
         <v>13</v>
@@ -5255,7 +5255,7 @@
         <v>224</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R48" s="3" t="s">
         <v>13</v>
@@ -5305,7 +5305,7 @@
         <v>346</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R49" s="3" t="s">
         <v>13</v>
@@ -5376,7 +5376,7 @@
         <v>203</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="R50" s="3" t="s">
         <v>13</v>
@@ -5423,7 +5423,7 @@
         <v>204</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R51" s="3" t="s">
         <v>13</v>
@@ -5494,7 +5494,7 @@
         <v>203</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R52" s="3" t="s">
         <v>13</v>
@@ -5562,7 +5562,7 @@
         <v>320</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="R53" s="3" t="s">
         <v>13</v>
@@ -5630,7 +5630,7 @@
         <v>320</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R54" s="3" t="s">
         <v>13</v>
@@ -5642,7 +5642,7 @@
         <v>195</v>
       </c>
       <c r="U54" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="V54" t="s">
         <v>190</v>
@@ -5704,7 +5704,7 @@
         <v>229</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R55" s="3" t="s">
         <v>13</v>
@@ -5775,7 +5775,7 @@
         <v>368</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R56" s="3" t="s">
         <v>13</v>
@@ -5846,7 +5846,7 @@
         <v>229</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R57" s="3" t="s">
         <v>13</v>
@@ -5899,7 +5899,7 @@
         <v>372</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q58" t="s">
         <v>371</v>
@@ -5952,13 +5952,13 @@
         <v>204</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>361</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>194</v>
@@ -5967,13 +5967,13 @@
         <v>201</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R59" s="3" t="s">
         <v>13</v>
@@ -6000,7 +6000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="80" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>155</v>
       </c>
@@ -6023,16 +6023,16 @@
         <v>204</v>
       </c>
       <c r="H60" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="I60" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>377</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>345</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>194</v>
@@ -6041,13 +6041,13 @@
         <v>201</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O60" s="3" t="s">
         <v>229</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="R60" s="3" t="s">
         <v>13</v>
@@ -6094,7 +6094,7 @@
         <v>204</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>361</v>
@@ -6103,7 +6103,7 @@
         <v>345</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R61" s="3" t="s">
         <v>13</v>
@@ -6159,7 +6159,7 @@
         <v>345</v>
       </c>
       <c r="K62" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>194</v>
@@ -6168,13 +6168,13 @@
         <v>195</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O62" s="3" t="s">
         <v>229</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R62" s="3" t="s">
         <v>13</v>
@@ -6230,7 +6230,7 @@
         <v>345</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L63" s="3" t="s">
         <v>194</v>
@@ -6239,13 +6239,13 @@
         <v>190</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O63" s="3" t="s">
         <v>224</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R63" s="3" t="s">
         <v>13</v>
@@ -6295,10 +6295,10 @@
         <v>1999</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R64" s="3" t="s">
         <v>13</v>
@@ -6345,7 +6345,7 @@
         <v>204</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R65" s="3" t="s">
         <v>13</v>
@@ -6369,7 +6369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="80" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>170</v>
       </c>
@@ -6389,10 +6389,10 @@
         <v>4</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>376</v>
+        <v>477</v>
       </c>
       <c r="I66" s="3">
         <v>1999</v>
@@ -6401,19 +6401,19 @@
         <v>345</v>
       </c>
       <c r="K66" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="M66" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N66" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="M66" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="N66" s="3" t="s">
+      <c r="O66" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="O66" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="P66" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q66" t="s">
         <v>371</v>
@@ -6469,7 +6469,7 @@
         <v>373</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>345</v>
@@ -6478,10 +6478,10 @@
         <v>194</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="R67" s="3" t="s">
         <v>13</v>
@@ -6528,22 +6528,22 @@
         <v>0</v>
       </c>
       <c r="G68" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="K68" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H68" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>397</v>
-      </c>
       <c r="P68" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>13</v>
@@ -6602,7 +6602,7 @@
         <v>345</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>194</v>
@@ -6611,13 +6611,13 @@
         <v>190</v>
       </c>
       <c r="N69" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="O69" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="O69" s="3" t="s">
-        <v>403</v>
-      </c>
       <c r="P69" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R69" s="3" t="s">
         <v>13</v>
@@ -6643,16 +6643,16 @@
     </row>
     <row r="70" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>412</v>
+      </c>
+      <c r="B70" t="s">
         <v>413</v>
-      </c>
-      <c r="B70" t="s">
-        <v>414</v>
       </c>
       <c r="C70">
         <v>2023</v>
       </c>
       <c r="D70" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E70">
         <v>37312405</v>
@@ -6661,10 +6661,10 @@
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="H70" s="3" t="s">
         <v>432</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>433</v>
       </c>
       <c r="I70" s="3">
         <v>2019</v>
@@ -6688,7 +6688,7 @@
         <v>229</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R70" s="7" t="s">
         <v>9</v>
@@ -6717,10 +6717,10 @@
     </row>
     <row r="71" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>414</v>
+      </c>
+      <c r="B71" t="s">
         <v>415</v>
-      </c>
-      <c r="B71" t="s">
-        <v>416</v>
       </c>
       <c r="C71">
         <v>2020</v>
@@ -6738,13 +6738,13 @@
         <v>204</v>
       </c>
       <c r="H71" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="J71" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="J71" s="3" t="s">
+      <c r="K71" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>436</v>
       </c>
       <c r="L71" s="3" t="s">
         <v>200</v>
@@ -6753,7 +6753,7 @@
         <v>190</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O71" s="3" t="s">
         <v>229</v>
@@ -6782,16 +6782,16 @@
     </row>
     <row r="72" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>416</v>
+      </c>
+      <c r="B72" t="s">
         <v>417</v>
-      </c>
-      <c r="B72" t="s">
-        <v>418</v>
       </c>
       <c r="C72">
         <v>2020</v>
       </c>
       <c r="D72" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E72">
         <v>32045058</v>
@@ -6832,10 +6832,10 @@
     </row>
     <row r="73" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>418</v>
+      </c>
+      <c r="B73" t="s">
         <v>419</v>
-      </c>
-      <c r="B73" t="s">
-        <v>420</v>
       </c>
       <c r="C73">
         <v>2020</v>
@@ -6853,16 +6853,16 @@
         <v>204</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I73" s="3">
         <v>2003</v>
       </c>
       <c r="J73" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="K73" s="3" t="s">
         <v>439</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>440</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>200</v>
@@ -6871,7 +6871,7 @@
         <v>201</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O73" s="3" t="s">
         <v>229</v>
@@ -6900,16 +6900,16 @@
     </row>
     <row r="74" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>420</v>
+      </c>
+      <c r="B74" t="s">
         <v>421</v>
-      </c>
-      <c r="B74" t="s">
-        <v>422</v>
       </c>
       <c r="C74">
         <v>2019</v>
       </c>
       <c r="D74" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E74">
         <v>31371748</v>
@@ -6921,13 +6921,13 @@
         <v>204</v>
       </c>
       <c r="H74" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="K74" s="3" t="s">
         <v>442</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>443</v>
       </c>
       <c r="L74" s="3" t="s">
         <v>200</v>
@@ -6936,7 +6936,7 @@
         <v>190</v>
       </c>
       <c r="N74" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="R74" s="7" t="s">
         <v>9</v>
@@ -6962,10 +6962,10 @@
     </row>
     <row r="75" spans="1:25" ht="176" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B75" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C75">
         <v>2016</v>
@@ -6983,22 +6983,22 @@
         <v>204</v>
       </c>
       <c r="H75" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="I75" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="J75" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="J75" s="3" t="s">
-        <v>446</v>
-      </c>
       <c r="K75" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="O75" s="3" t="s">
         <v>203</v>
       </c>
       <c r="Q75" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="R75" s="7" t="s">
         <v>9</v>
@@ -7024,10 +7024,10 @@
     </row>
     <row r="76" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>471</v>
+      </c>
+      <c r="B76" t="s">
         <v>472</v>
-      </c>
-      <c r="B76" t="s">
-        <v>473</v>
       </c>
       <c r="C76">
         <v>2009</v>
@@ -7042,10 +7042,10 @@
         <v>204</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>194</v>
@@ -7054,13 +7054,13 @@
         <v>190</v>
       </c>
       <c r="N76" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q76" t="s">
         <v>476</v>
-      </c>
-      <c r="O76" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>477</v>
       </c>
       <c r="R76" s="7" t="s">
         <v>9</v>
@@ -7089,16 +7089,16 @@
     </row>
     <row r="77" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>462</v>
+      </c>
+      <c r="B77" t="s">
         <v>463</v>
-      </c>
-      <c r="B77" t="s">
-        <v>464</v>
       </c>
       <c r="C77">
         <v>2018</v>
       </c>
       <c r="D77" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E77">
         <v>32288829</v>
@@ -7113,7 +7113,7 @@
         <v>195</v>
       </c>
       <c r="U77" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="V77" t="s">
         <v>195</v>
@@ -7127,16 +7127,16 @@
     </row>
     <row r="78" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>464</v>
+      </c>
+      <c r="B78" t="s">
         <v>465</v>
-      </c>
-      <c r="B78" t="s">
-        <v>466</v>
       </c>
       <c r="C78">
         <v>2003</v>
       </c>
       <c r="D78" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E78">
         <v>12722231</v>
@@ -7151,7 +7151,7 @@
         <v>195</v>
       </c>
       <c r="U78" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="V78" t="s">
         <v>195</v>

</xml_diff>